<commit_message>
ajuste no regex de atas de grupos + itens
</commit_message>
<xml_diff>
--- a/controle_contratos/Planilha_Completa.xlsx
+++ b/controle_contratos/Planilha_Completa.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1705" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1709" uniqueCount="376">
   <si>
     <t>Nº</t>
   </si>
@@ -597,6 +597,12 @@
     <t>14/02/2028</t>
   </si>
   <si>
+    <t>https://www.com7dn.mb/sites/default/arquivos/obtencao/Atas_e_Contratos/PE_08-2023/87000_24-002_00/contrato_inicial/contrato_inicial.pdf</t>
+  </si>
+  <si>
+    <t>https://www.com7dn.mb/sites/default/arquivos/obtencao/Atas_e_Contratos/PE_10-2020/87000_21-005_00/contrato_inicial/contrato_inicial.pdf</t>
+  </si>
+  <si>
     <t>Centro de Intendência da Marinha em Brasília</t>
   </si>
   <si>
@@ -606,10 +612,13 @@
     <t>Controle de Contratos - 2024</t>
   </si>
   <si>
-    <t>Atualizado em: 12/03/2024</t>
+    <t>Atualizado em: 13/03/2024</t>
   </si>
   <si>
     <t>Link indisponível</t>
+  </si>
+  <si>
+    <t>Ver Detalhes</t>
   </si>
   <si>
     <t>Ata</t>
@@ -1141,7 +1150,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1180,6 +1189,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1220,10 +1236,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1237,8 +1257,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1554,7 +1576,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="20" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1569,7 +1591,7 @@
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1584,7 +1606,7 @@
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1599,7 +1621,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1668,10 +1690,10 @@
         <v>162</v>
       </c>
       <c r="I6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1698,10 +1720,10 @@
         <v>163</v>
       </c>
       <c r="I7" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1730,10 +1752,10 @@
         <v>164</v>
       </c>
       <c r="I8" s="4">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1762,10 +1784,10 @@
         <v>165</v>
       </c>
       <c r="I9" s="4">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1794,10 +1816,10 @@
         <v>166</v>
       </c>
       <c r="I10" s="4">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1826,10 +1848,10 @@
         <v>167</v>
       </c>
       <c r="I11" s="4">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1858,10 +1880,10 @@
         <v>168</v>
       </c>
       <c r="I12" s="4">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1890,10 +1912,10 @@
         <v>169</v>
       </c>
       <c r="I13" s="4">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1922,10 +1944,10 @@
         <v>170</v>
       </c>
       <c r="I14" s="4">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1954,10 +1976,10 @@
         <v>170</v>
       </c>
       <c r="I15" s="4">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1986,10 +2008,10 @@
         <v>171</v>
       </c>
       <c r="I16" s="4">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -2018,10 +2040,10 @@
         <v>171</v>
       </c>
       <c r="I17" s="4">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -2050,10 +2072,10 @@
         <v>171</v>
       </c>
       <c r="I18" s="4">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -2082,10 +2104,10 @@
         <v>172</v>
       </c>
       <c r="I19" s="4">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -2114,10 +2136,10 @@
         <v>173</v>
       </c>
       <c r="I20" s="4">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -2146,10 +2168,10 @@
         <v>174</v>
       </c>
       <c r="I21" s="4">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -2178,10 +2200,10 @@
         <v>175</v>
       </c>
       <c r="I22" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -2210,10 +2232,10 @@
         <v>176</v>
       </c>
       <c r="I23" s="4">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -2242,10 +2264,10 @@
         <v>177</v>
       </c>
       <c r="I24" s="4">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -2274,10 +2296,10 @@
         <v>178</v>
       </c>
       <c r="I25" s="4">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -2306,10 +2328,10 @@
         <v>179</v>
       </c>
       <c r="I26" s="4">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -2338,10 +2360,10 @@
         <v>180</v>
       </c>
       <c r="I27" s="4">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -2370,10 +2392,10 @@
         <v>181</v>
       </c>
       <c r="I28" s="4">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -2402,10 +2424,10 @@
         <v>181</v>
       </c>
       <c r="I29" s="4">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -2434,10 +2456,10 @@
         <v>182</v>
       </c>
       <c r="I30" s="4">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -2466,10 +2488,10 @@
         <v>183</v>
       </c>
       <c r="I31" s="4">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -2498,10 +2520,10 @@
         <v>184</v>
       </c>
       <c r="I32" s="4">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2530,10 +2552,10 @@
         <v>184</v>
       </c>
       <c r="I33" s="4">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2562,10 +2584,10 @@
         <v>184</v>
       </c>
       <c r="I34" s="4">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -2594,10 +2616,10 @@
         <v>184</v>
       </c>
       <c r="I35" s="4">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -2626,10 +2648,10 @@
         <v>185</v>
       </c>
       <c r="I36" s="4">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -2658,10 +2680,10 @@
         <v>186</v>
       </c>
       <c r="I37" s="4">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2690,10 +2712,10 @@
         <v>187</v>
       </c>
       <c r="I38" s="4">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2722,10 +2744,10 @@
         <v>187</v>
       </c>
       <c r="I39" s="4">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2754,10 +2776,10 @@
         <v>188</v>
       </c>
       <c r="I40" s="4">
-        <v>347</v>
-      </c>
-      <c r="J40" s="4" t="s">
-        <v>197</v>
+        <v>346</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2786,10 +2808,10 @@
         <v>189</v>
       </c>
       <c r="I41" s="4">
-        <v>353</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>197</v>
+        <v>352</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2818,10 +2840,10 @@
         <v>190</v>
       </c>
       <c r="I42" s="4">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2848,10 +2870,10 @@
         <v>191</v>
       </c>
       <c r="I43" s="4">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2880,10 +2902,10 @@
         <v>191</v>
       </c>
       <c r="I44" s="4">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2912,10 +2934,10 @@
         <v>192</v>
       </c>
       <c r="I45" s="4">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2925,6 +2947,10 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="J40" r:id="rId1"/>
+    <hyperlink ref="J41" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0" right="0" top="0" bottom="0.7" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape"/>
 </worksheet>
@@ -2955,7 +2981,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="20" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2970,7 +2996,7 @@
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2985,7 +3011,7 @@
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3000,7 +3026,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -3021,7 +3047,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>3</v>
@@ -3050,10 +3076,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>79</v>
@@ -3062,19 +3088,19 @@
         <v>82</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="I6" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -3082,10 +3108,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>79</v>
@@ -3094,19 +3120,19 @@
         <v>82</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="I7" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -3114,31 +3140,31 @@
         <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>80</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="I8" s="4">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -3146,31 +3172,31 @@
         <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>80</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="I9" s="4">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -3178,31 +3204,31 @@
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>80</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="I10" s="4">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -3210,31 +3236,31 @@
         <v>6</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>80</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="I11" s="4">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -3242,31 +3268,31 @@
         <v>7</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>80</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="I12" s="4">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -3274,31 +3300,31 @@
         <v>8</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>80</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="I13" s="4">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -3306,31 +3332,31 @@
         <v>9</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>80</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="I14" s="4">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -3338,31 +3364,31 @@
         <v>10</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>80</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="I15" s="4">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -3370,31 +3396,31 @@
         <v>11</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>80</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="I16" s="4">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -3402,31 +3428,31 @@
         <v>12</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>80</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="I17" s="4">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -3434,31 +3460,31 @@
         <v>13</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>80</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="I18" s="4">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -3466,31 +3492,31 @@
         <v>14</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>80</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="I19" s="4">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -3498,31 +3524,31 @@
         <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>80</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="I20" s="4">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -3533,7 +3559,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>79</v>
@@ -3542,19 +3568,19 @@
         <v>82</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>140</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="I21" s="4">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -3565,7 +3591,7 @@
         <v>35</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>80</v>
@@ -3577,16 +3603,16 @@
         <v>130</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>169</v>
       </c>
       <c r="I22" s="4">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -3597,7 +3623,7 @@
         <v>16</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>79</v>
@@ -3606,19 +3632,19 @@
         <v>82</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>140</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="I23" s="4">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -3629,7 +3655,7 @@
         <v>16</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>79</v>
@@ -3638,19 +3664,19 @@
         <v>82</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>140</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="I24" s="4">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -3661,7 +3687,7 @@
         <v>16</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>79</v>
@@ -3670,19 +3696,19 @@
         <v>82</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>140</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="I25" s="4">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -3693,7 +3719,7 @@
         <v>16</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>79</v>
@@ -3702,19 +3728,19 @@
         <v>82</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>140</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="I26" s="4">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -3725,7 +3751,7 @@
         <v>16</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>79</v>
@@ -3734,19 +3760,19 @@
         <v>82</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>140</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="I27" s="4">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -3757,7 +3783,7 @@
         <v>16</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>79</v>
@@ -3766,19 +3792,19 @@
         <v>82</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>140</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="I28" s="4">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -3789,7 +3815,7 @@
         <v>16</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>79</v>
@@ -3798,19 +3824,19 @@
         <v>82</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>140</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="I29" s="4">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -3821,7 +3847,7 @@
         <v>16</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>79</v>
@@ -3830,19 +3856,19 @@
         <v>82</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>140</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="I30" s="4">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -3850,31 +3876,31 @@
         <v>26</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>80</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="I31" s="4">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -3882,10 +3908,10 @@
         <v>27</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>79</v>
@@ -3894,19 +3920,19 @@
         <v>82</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>140</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="I32" s="4">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -3914,10 +3940,10 @@
         <v>28</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>79</v>
@@ -3926,19 +3952,19 @@
         <v>82</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="I33" s="4">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -3946,10 +3972,10 @@
         <v>29</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>79</v>
@@ -3958,19 +3984,19 @@
         <v>82</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="I34" s="4">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -3978,10 +4004,10 @@
         <v>30</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>79</v>
@@ -3993,16 +4019,16 @@
         <v>128</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="I35" s="4">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -4010,10 +4036,10 @@
         <v>31</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>79</v>
@@ -4022,19 +4048,19 @@
         <v>82</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="I36" s="4">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -4042,10 +4068,10 @@
         <v>32</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>79</v>
@@ -4054,19 +4080,19 @@
         <v>82</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="I37" s="4">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -4074,10 +4100,10 @@
         <v>33</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>79</v>
@@ -4086,19 +4112,19 @@
         <v>82</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="I38" s="4">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -4106,10 +4132,10 @@
         <v>34</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>79</v>
@@ -4118,19 +4144,19 @@
         <v>82</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="I39" s="4">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -4138,10 +4164,10 @@
         <v>35</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>79</v>
@@ -4150,19 +4176,19 @@
         <v>82</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="I40" s="4">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -4170,10 +4196,10 @@
         <v>36</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>79</v>
@@ -4182,19 +4208,19 @@
         <v>82</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="I41" s="4">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -4202,10 +4228,10 @@
         <v>37</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>79</v>
@@ -4217,16 +4243,16 @@
         <v>128</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="I42" s="4">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -4237,7 +4263,7 @@
         <v>21</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>80</v>
@@ -4255,10 +4281,10 @@
         <v>173</v>
       </c>
       <c r="I43" s="4">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -4269,28 +4295,28 @@
         <v>24</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>79</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>148</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="I44" s="4">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -4301,7 +4327,7 @@
         <v>24</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>80</v>
@@ -4310,19 +4336,19 @@
         <v>90</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>148</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="I45" s="4">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -4333,7 +4359,7 @@
         <v>24</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>80</v>
@@ -4342,19 +4368,19 @@
         <v>90</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>148</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="I46" s="4">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -4365,7 +4391,7 @@
         <v>24</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>80</v>
@@ -4374,19 +4400,19 @@
         <v>90</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>148</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="I47" s="4">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -4397,7 +4423,7 @@
         <v>24</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>80</v>
@@ -4406,19 +4432,19 @@
         <v>90</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>148</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="I48" s="4">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -4429,7 +4455,7 @@
         <v>24</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>80</v>
@@ -4444,13 +4470,13 @@
         <v>148</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="I49" s="4">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -4461,7 +4487,7 @@
         <v>24</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>80</v>
@@ -4470,19 +4496,19 @@
         <v>90</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>148</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="I50" s="4">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -4493,7 +4519,7 @@
         <v>24</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>80</v>
@@ -4502,19 +4528,19 @@
         <v>90</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>148</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="I51" s="4">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -4525,7 +4551,7 @@
         <v>24</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>80</v>
@@ -4534,19 +4560,19 @@
         <v>90</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>148</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="I52" s="4">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -4557,7 +4583,7 @@
         <v>24</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>80</v>
@@ -4566,19 +4592,19 @@
         <v>90</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>148</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="I53" s="4">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -4589,7 +4615,7 @@
         <v>24</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>80</v>
@@ -4598,19 +4624,19 @@
         <v>90</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>148</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="I54" s="4">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -4621,7 +4647,7 @@
         <v>24</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>80</v>
@@ -4630,19 +4656,19 @@
         <v>90</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>148</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="I55" s="4">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -4650,29 +4676,29 @@
         <v>51</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="I56" s="4">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -4680,10 +4706,10 @@
         <v>52</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>80</v>
@@ -4692,19 +4718,19 @@
         <v>91</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>148</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="I57" s="4">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -4712,10 +4738,10 @@
         <v>53</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>79</v>
@@ -4724,19 +4750,19 @@
         <v>82</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="I58" s="4">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -4744,10 +4770,10 @@
         <v>54</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>79</v>
@@ -4756,19 +4782,19 @@
         <v>82</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="I59" s="4">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -4776,10 +4802,10 @@
         <v>55</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>79</v>
@@ -4788,19 +4814,19 @@
         <v>82</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="I60" s="4">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -4808,10 +4834,10 @@
         <v>56</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>79</v>
@@ -4820,19 +4846,19 @@
         <v>82</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="I61" s="4">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -4840,10 +4866,10 @@
         <v>57</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>79</v>
@@ -4852,19 +4878,19 @@
         <v>82</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="I62" s="4">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -4872,10 +4898,10 @@
         <v>58</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>79</v>
@@ -4884,19 +4910,19 @@
         <v>82</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="I63" s="4">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -4904,10 +4930,10 @@
         <v>59</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>79</v>
@@ -4916,19 +4942,19 @@
         <v>82</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="I64" s="4">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -4936,10 +4962,10 @@
         <v>60</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>79</v>
@@ -4948,19 +4974,19 @@
         <v>82</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="I65" s="4">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -4968,10 +4994,10 @@
         <v>61</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>79</v>
@@ -4980,19 +5006,19 @@
         <v>82</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="I66" s="4">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -5000,10 +5026,10 @@
         <v>62</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>79</v>
@@ -5012,19 +5038,19 @@
         <v>82</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="I67" s="4">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -5032,10 +5058,10 @@
         <v>63</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>79</v>
@@ -5044,19 +5070,19 @@
         <v>82</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="I68" s="4">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -5064,10 +5090,10 @@
         <v>64</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>79</v>
@@ -5076,19 +5102,19 @@
         <v>82</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="H69" s="4" t="s">
         <v>183</v>
       </c>
       <c r="I69" s="4">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -5096,10 +5122,10 @@
         <v>65</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>79</v>
@@ -5108,19 +5134,19 @@
         <v>82</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="I70" s="4">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -5128,10 +5154,10 @@
         <v>66</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>79</v>
@@ -5140,19 +5166,19 @@
         <v>82</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="I71" s="4">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -5160,10 +5186,10 @@
         <v>67</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>79</v>
@@ -5172,19 +5198,19 @@
         <v>82</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="I72" s="4">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -5192,10 +5218,10 @@
         <v>68</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>79</v>
@@ -5204,19 +5230,19 @@
         <v>82</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="I73" s="4">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -5224,10 +5250,10 @@
         <v>69</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>79</v>
@@ -5236,19 +5262,19 @@
         <v>82</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="I74" s="4">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -5256,10 +5282,10 @@
         <v>70</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>79</v>
@@ -5268,19 +5294,19 @@
         <v>82</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="I75" s="4">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -5291,7 +5317,7 @@
         <v>25</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>80</v>
@@ -5300,19 +5326,19 @@
         <v>84</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>157</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="I76" s="4">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>